<commit_message>
fixed order, and phi distribution of particles
</commit_message>
<xml_diff>
--- a/benchmarks/template.xlsx
+++ b/benchmarks/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/projects/gemc/clas12Tags/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0773E6F-5B5E-6648-B157-85487FF47102}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC7A941-35BF-FB4E-9539-54FF9A6F5EA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25060" yWindow="3840" windowWidth="32580" windowHeight="31240" xr2:uid="{28AA30A8-E2EF-AD44-AC50-0F7BDEF7D56D}"/>
+    <workbookView xWindow="11820" yWindow="2580" windowWidth="32580" windowHeight="31240" xr2:uid="{28AA30A8-E2EF-AD44-AC50-0F7BDEF7D56D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -160,11 +160,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,7 +483,7 @@
   <dimension ref="C2:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,23 +496,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -559,19 +559,19 @@
         <v>20</v>
       </c>
       <c r="D7" s="1">
-        <v>1.7575799999999999</v>
-      </c>
-      <c r="E7" s="5">
-        <f>1000*D7/$D$4</f>
-        <v>0.87878999999999996</v>
-      </c>
-      <c r="F7" s="5">
-        <f>$D$4/D7</f>
-        <v>1137.9282877593055</v>
+        <v>5.9450000000000003</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" ref="E7:E21" si="0">1000*D7/$D$4</f>
+        <v>1.1890000000000001</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" ref="F7:F21" si="1">$D$4/D7</f>
+        <v>841.04289318755252</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ref="G7:G21" si="0">D7/D$21</f>
-        <v>1.7614163648426271E-3</v>
+        <f t="shared" ref="G7:G21" si="2">D7/D$21</f>
+        <v>2.2978776037137104E-3</v>
       </c>
       <c r="H7" s="1" t="str">
         <f>C7</f>
@@ -579,11 +579,11 @@
       </c>
       <c r="I7" s="1">
         <f>D7</f>
-        <v>1.7575799999999999</v>
+        <v>5.9450000000000003</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" ref="J7:J21" si="1">I7/$I$21</f>
-        <v>5.1862540278318743E-3</v>
+        <f>I7/$D$21</f>
+        <v>2.2978776037137104E-3</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -593,31 +593,31 @@
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>3.4910000000000001</v>
-      </c>
-      <c r="E8" s="5">
-        <f>1000*D8/$D$4</f>
-        <v>1.7455000000000001</v>
-      </c>
-      <c r="F8" s="5">
-        <f>$D$4/D8</f>
-        <v>572.9017473503294</v>
+        <v>10.420299999999999</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>2.08406</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>479.8326343771293</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>3.4986199943476894E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.0276827576077329E-3</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f>C8</f>
+        <f t="shared" ref="H8:H21" si="3">C8</f>
         <v>svt</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8:I21" si="2">D8-D7</f>
-        <v>1.7334200000000002</v>
+        <f t="shared" ref="I8:I21" si="4">D8-D7</f>
+        <v>4.4752999999999989</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="1"/>
-        <v>5.1149628790293066E-3</v>
+        <f>I8/$D$21</f>
+        <v>1.7298051538940228E-3</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -627,31 +627,31 @@
         <v>7</v>
       </c>
       <c r="D9" s="1">
-        <v>3.8567</v>
-      </c>
-      <c r="E9" s="5">
-        <f>1000*D9/$D$4</f>
-        <v>1.92835</v>
-      </c>
-      <c r="F9" s="5">
-        <f>$D$4/D9</f>
-        <v>518.57805896232526</v>
+        <v>11.6716</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>2.33432</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>428.39028068131194</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>3.8651182274994939E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.5113386441555832E-3</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f>C9</f>
+        <f t="shared" si="3"/>
         <v>ctof</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="2"/>
-        <v>0.36569999999999991</v>
+        <f t="shared" si="4"/>
+        <v>1.2513000000000005</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0791048475620548E-3</v>
+        <f>I9/$D$21</f>
+        <v>4.8365588654784977E-4</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -661,31 +661,31 @@
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>4.4462999999999999</v>
-      </c>
-      <c r="E10" s="5">
-        <f>1000*D10/$D$4</f>
-        <v>2.22315</v>
-      </c>
-      <c r="F10" s="5">
-        <f>$D$4/D10</f>
-        <v>449.81220340507838</v>
+        <v>12.524800000000001</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>2.5049600000000001</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>399.20797138477258</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>4.4560051792804731E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.8411198336406188E-3</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f>C10</f>
+        <f t="shared" si="3"/>
         <v>cnd</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.5895999999999999</v>
+        <f t="shared" si="4"/>
+        <v>0.85320000000000107</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7397873068706248E-3</v>
+        <f>I10/$D$21</f>
+        <v>3.2978118948503619E-4</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -695,31 +695,31 @@
         <v>9</v>
       </c>
       <c r="D11" s="1">
-        <v>71.590800000000002</v>
-      </c>
-      <c r="E11" s="5">
-        <f>1000*D11/$D$4</f>
-        <v>35.795400000000001</v>
-      </c>
-      <c r="F11" s="5">
-        <f>$D$4/D11</f>
-        <v>27.93655050648966</v>
+        <v>181.00299999999999</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>36.200600000000001</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>27.623851538372293</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>7.1747065107804806E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.9961772902437797E-2</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f>C11</f>
+        <f t="shared" si="3"/>
         <v>solenoid</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="2"/>
-        <v>67.144500000000008</v>
+        <f t="shared" si="4"/>
+        <v>168.47819999999999</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.19812949258170745</v>
+        <f>I11/$D$21</f>
+        <v>6.5120653068797177E-2</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -729,31 +729,31 @@
         <v>10</v>
       </c>
       <c r="D12" s="1">
-        <v>123.345</v>
-      </c>
-      <c r="E12" s="5">
-        <f>1000*D12/$D$4</f>
-        <v>61.672499999999999</v>
-      </c>
-      <c r="F12" s="5">
-        <f>$D$4/D12</f>
-        <v>16.214682394908589</v>
+        <v>288.33</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>57.665999999999997</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>17.341240939201612</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.12361423179685355</v>
+        <f t="shared" si="2"/>
+        <v>0.11144609747330093</v>
       </c>
       <c r="H12" s="1" t="str">
-        <f>C12</f>
+        <f t="shared" si="3"/>
         <v>mm</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="2"/>
-        <v>51.754199999999997</v>
+        <f t="shared" si="4"/>
+        <v>107.327</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.15271590949328986</v>
+        <f>I12/$D$21</f>
+        <v>4.1484324570863144E-2</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -763,31 +763,31 @@
         <v>11</v>
       </c>
       <c r="D13" s="1">
-        <v>172.43700000000001</v>
-      </c>
-      <c r="E13" s="5">
-        <f>1000*D13/$D$4</f>
-        <v>86.218500000000006</v>
-      </c>
-      <c r="F13" s="5">
-        <f>$D$4/D13</f>
-        <v>11.598438850130771</v>
+        <v>414.76299999999998</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>82.952600000000004</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="1"/>
+        <v>12.055077236879857</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17281338755810155</v>
+        <f t="shared" si="2"/>
+        <v>0.16031532523954745</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>C13</f>
+        <f t="shared" si="3"/>
         <v>htcc</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="2"/>
-        <v>49.092000000000013</v>
+        <f t="shared" si="4"/>
+        <v>126.43299999999999</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.14486030947912612</v>
+        <f>I13/$D$21</f>
+        <v>4.8869227766246512E-2</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -797,99 +797,99 @@
         <v>12</v>
       </c>
       <c r="D14" s="1">
-        <v>278.654</v>
-      </c>
-      <c r="E14" s="5">
-        <f>1000*D14/$D$4</f>
-        <v>139.327</v>
-      </c>
-      <c r="F14" s="5">
-        <f>$D$4/D14</f>
-        <v>7.1773597364473503</v>
+        <v>624.875</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>124.97499999999999</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>8.0016003200640125</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.27926223314378718</v>
+        <f t="shared" si="2"/>
+        <v>0.24152838816158195</v>
       </c>
       <c r="H14" s="1" t="str">
-        <f>C14</f>
+        <f t="shared" si="3"/>
         <v>ft</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="2"/>
-        <v>106.21699999999998</v>
+        <f t="shared" si="4"/>
+        <v>210.11200000000002</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31342433577658951</v>
+        <f>I14/$D$21</f>
+        <v>8.1213062922034507E-2</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1">
-        <v>166.35499999999999</v>
-      </c>
-      <c r="E15" s="5">
-        <f>1000*D15/$D$4</f>
-        <v>83.177499999999995</v>
-      </c>
-      <c r="F15" s="5">
-        <f>$D$4/D15</f>
-        <v>12.022482041417451</v>
+        <v>579.625</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>115.925</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>8.6262669829631236</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.16671811204804063</v>
+        <f t="shared" si="2"/>
+        <v>0.22403823482801671</v>
       </c>
       <c r="H15" s="1" t="str">
-        <f>C15</f>
-        <v>torus</v>
+        <f t="shared" si="3"/>
+        <v>dc</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="2"/>
-        <v>-112.29900000000001</v>
+        <f t="shared" si="4"/>
+        <v>-45.25</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.33137105626571295</v>
+        <f>I15/$D$21</f>
+        <v>-1.7490153333565246E-2</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1">
-        <v>238.61699999999999</v>
-      </c>
-      <c r="E16" s="5">
-        <f>1000*D16/$D$4</f>
-        <v>119.3085</v>
-      </c>
-      <c r="F16" s="5">
-        <f>$D$4/D16</f>
-        <v>8.381632490560186</v>
+        <v>594.04499999999996</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>118.809</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>8.4168707757829804</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.23913784222035592</v>
+        <f t="shared" si="2"/>
+        <v>0.22961189253122136</v>
       </c>
       <c r="H16" s="1" t="str">
-        <f>C16</f>
-        <v>dc</v>
+        <f t="shared" si="3"/>
+        <v>torus</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="2"/>
-        <v>72.262</v>
+        <f t="shared" si="4"/>
+        <v>14.419999999999959</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21323017362463553</v>
+        <f>I16/$D$21</f>
+        <v>5.5736577032046439E-3</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -899,31 +899,31 @@
         <v>15</v>
       </c>
       <c r="D17" s="1">
-        <v>258.40800000000002</v>
-      </c>
-      <c r="E17" s="5">
-        <f>1000*D17/$D$4</f>
-        <v>129.20400000000001</v>
-      </c>
-      <c r="F17" s="5">
-        <f>$D$4/D17</f>
-        <v>7.7396984613479454</v>
+        <v>590.26400000000001</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>118.0528</v>
+      </c>
+      <c r="F17" s="4">
+        <f t="shared" si="1"/>
+        <v>8.4707859534039009</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.25897204110552785</v>
+        <f t="shared" si="2"/>
+        <v>0.22815045010571397</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f>C17</f>
+        <f t="shared" si="3"/>
         <v>ltcc</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="2"/>
-        <v>19.791000000000025</v>
+        <f t="shared" si="4"/>
+        <v>-3.7809999999999491</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="1"/>
-        <v>5.8399136007931798E-2</v>
+        <f>I17/$D$21</f>
+        <v>-1.4614424255073881E-3</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -933,31 +933,31 @@
         <v>16</v>
       </c>
       <c r="D18" s="1">
-        <v>263.19</v>
-      </c>
-      <c r="E18" s="5">
-        <f>1000*D18/$D$4</f>
-        <v>131.595</v>
-      </c>
-      <c r="F18" s="5">
-        <f>$D$4/D18</f>
-        <v>7.5990729131046013</v>
+        <v>603.63</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>120.726</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="1"/>
+        <v>8.283219853221345</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.26376447903533895</v>
+        <f t="shared" si="2"/>
+        <v>0.23331671285613237</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f>C18</f>
+        <f t="shared" si="3"/>
         <v>rich</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="2"/>
-        <v>4.7819999999999823</v>
+        <f t="shared" si="4"/>
+        <v>13.365999999999985</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4110690131369232E-2</v>
+        <f>I18/$D$21</f>
+        <v>5.166262750418405E-3</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -967,31 +967,31 @@
         <v>17</v>
       </c>
       <c r="D19" s="1">
-        <v>278.654</v>
-      </c>
-      <c r="E19" s="5">
-        <f>1000*D19/$D$4</f>
-        <v>139.327</v>
-      </c>
-      <c r="F19" s="5">
-        <f>$D$4/D19</f>
-        <v>7.1773597364473503</v>
+        <v>624.875</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>124.97499999999999</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="1"/>
+        <v>8.0016003200640125</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.27926223314378718</v>
+        <f t="shared" si="2"/>
+        <v>0.24152838816158195</v>
       </c>
       <c r="H19" s="1" t="str">
-        <f>C19</f>
+        <f t="shared" si="3"/>
         <v>ftof</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="2"/>
-        <v>15.463999999999999</v>
+        <f t="shared" si="4"/>
+        <v>21.245000000000005</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="1"/>
-        <v>4.5631056501776367E-2</v>
+        <f>I19/$D$21</f>
+        <v>8.2116753054495856E-3</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1001,31 +1001,31 @@
         <v>18</v>
       </c>
       <c r="D20" s="1">
-        <v>658.93</v>
-      </c>
-      <c r="E20" s="5">
-        <f>1000*D20/$D$4</f>
-        <v>329.46499999999997</v>
-      </c>
-      <c r="F20" s="5">
-        <f>$D$4/D20</f>
-        <v>3.0352237718725816</v>
+        <v>1586.6</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>317.32</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="1"/>
+        <v>3.1513929156687257</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.66036828211845389</v>
+        <f t="shared" si="2"/>
+        <v>0.61325695644275402</v>
       </c>
       <c r="H20" s="1" t="str">
-        <f>C20</f>
+        <f t="shared" si="3"/>
         <v>pcal</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="2"/>
-        <v>380.27599999999995</v>
+        <f t="shared" si="4"/>
+        <v>961.72499999999991</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="1"/>
-        <v>1.1221156002502268</v>
+        <f>I20/$D$21</f>
+        <v>0.37172856828117207</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1035,31 +1035,31 @@
         <v>19</v>
       </c>
       <c r="D21" s="1">
-        <v>997.822</v>
-      </c>
-      <c r="E21" s="5">
-        <f>1000*D21/$D$4</f>
-        <v>498.911</v>
-      </c>
-      <c r="F21" s="5">
-        <f>$D$4/D21</f>
-        <v>2.004365508076591</v>
+        <v>2587.17</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>517.43399999999997</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>1.9326136280182593</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H21" s="1" t="str">
-        <f>C21</f>
+        <f t="shared" si="3"/>
         <v>ecAll</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="2"/>
-        <v>338.89200000000005</v>
+        <f t="shared" si="4"/>
+        <v>1000.5700000000002</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>I21/$D$21</f>
+        <v>0.38674304355724598</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>

</xml_diff>

<commit_message>
results with 4.3.2, fixed ft reporting
</commit_message>
<xml_diff>
--- a/benchmarks/template.xlsx
+++ b/benchmarks/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/projects/gemc/clas12Tags/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E0B52A-D39D-4545-A3DE-6E62825201C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7DC960-D85F-4245-B0E4-63A45C84DF13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15880" yWindow="1320" windowWidth="44280" windowHeight="31240" xr2:uid="{28AA30A8-E2EF-AD44-AC50-0F7BDEF7D56D}"/>
+    <workbookView xWindow="10040" yWindow="2780" windowWidth="44280" windowHeight="31240" xr2:uid="{28AA30A8-E2EF-AD44-AC50-0F7BDEF7D56D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,13 +219,16 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -546,7 +549,7 @@
   <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,19 +565,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="2:14" ht="26" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -590,10 +593,10 @@
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -602,21 +605,21 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="1">
-        <v>5000</v>
-      </c>
-      <c r="F5" s="8">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="7">
         <f>SUM(F9:F23)</f>
-        <v>8422.0725600000005</v>
-      </c>
-      <c r="G5" s="8">
+        <v>25251.930499999999</v>
+      </c>
+      <c r="G5" s="7">
         <f>F5/3600</f>
-        <v>2.3394646000000003</v>
+        <v>7.0144251388888881</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -641,19 +644,19 @@
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
@@ -694,43 +697,43 @@
         <v>19</v>
       </c>
       <c r="C9" s="1">
-        <v>0.60707199999999994</v>
+        <v>11.889099999999999</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" ref="D9:D23" si="0">1000*C9/$C$5</f>
-        <v>1.2141439999999997</v>
+        <v>1.1889099999999999</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" ref="E9:E23" si="1">$C$5/C9</f>
-        <v>823.62553370934597</v>
+        <v>841.10655979005992</v>
       </c>
       <c r="F9" s="5">
-        <f>D9*$E$5/1000</f>
-        <v>6.0707199999999988</v>
+        <f t="shared" ref="F9:F23" si="2">D9*$E$5/1000</f>
+        <v>11.889099999999999</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" ref="G9:G23" si="2">C9/C$23</f>
-        <v>2.514536605571088E-3</v>
+        <f>C9/C$23</f>
+        <v>2.0666308585771671E-3</v>
       </c>
       <c r="H9" s="1">
         <f>C9</f>
-        <v>0.60707199999999994</v>
+        <v>11.889099999999999</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>B9</f>
+        <f t="shared" ref="I9:I23" si="3">B9</f>
         <v>target</v>
       </c>
       <c r="J9" s="5">
-        <f>1000/K9</f>
-        <v>823.62553370934609</v>
+        <f t="shared" ref="J9:J23" si="4">1000/K9</f>
+        <v>841.10655979005992</v>
       </c>
       <c r="K9" s="5">
         <f>D9</f>
-        <v>1.2141439999999997</v>
+        <v>1.1889099999999999</v>
       </c>
       <c r="L9" s="2">
         <f>H9/$C$23</f>
-        <v>2.514536605571088E-3</v>
+        <v>2.0666308585771671E-3</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -740,43 +743,43 @@
         <v>5</v>
       </c>
       <c r="C10" s="1">
-        <v>0.97791399999999995</v>
+        <v>20.143899999999999</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="0"/>
-        <v>1.9558279999999999</v>
+        <v>2.0143899999999997</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="1"/>
-        <v>511.2924040355287</v>
+        <v>496.42819910742213</v>
       </c>
       <c r="F10" s="5">
-        <f>D10*$E$5/1000</f>
-        <v>9.7791399999999999</v>
+        <f t="shared" si="2"/>
+        <v>20.143899999999999</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="2"/>
-        <v>4.0505912809361078E-3</v>
+        <f>C10/C$23</f>
+        <v>3.5015270585740379E-3</v>
       </c>
       <c r="H10" s="1">
-        <f>C10-C9</f>
-        <v>0.370842</v>
+        <f t="shared" ref="H10:H23" si="5">C10-C9</f>
+        <v>8.2547999999999995</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>B10</f>
+        <f t="shared" si="3"/>
         <v>svt</v>
       </c>
       <c r="J10" s="5">
-        <f>1000/K10</f>
-        <v>1348.2830963051647</v>
+        <f t="shared" si="4"/>
+        <v>1211.4163880408978</v>
       </c>
       <c r="K10" s="5">
-        <f>D10-D9</f>
-        <v>0.74168400000000023</v>
+        <f t="shared" ref="K10:K23" si="6">D10-D9</f>
+        <v>0.82547999999999977</v>
       </c>
       <c r="L10" s="2">
         <f>H10/$C$23</f>
-        <v>1.5360546753650202E-3</v>
+        <v>1.434896199996871E-3</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -786,43 +789,43 @@
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>1.2085699999999999</v>
+        <v>24.051400000000001</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="0"/>
-        <v>2.4171399999999998</v>
+        <v>2.4051400000000003</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="1"/>
-        <v>413.71207294571275</v>
+        <v>415.77621261132407</v>
       </c>
       <c r="F11" s="5">
-        <f>D11*$E$5/1000</f>
-        <v>12.085699999999999</v>
+        <f t="shared" si="2"/>
+        <v>24.051400000000001</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="2"/>
-        <v>5.0059852956404671E-3</v>
+        <f>C11/C$23</f>
+        <v>4.1807508921602879E-3</v>
       </c>
       <c r="H11" s="1">
-        <f>C11-C10</f>
-        <v>0.23065599999999997</v>
+        <f t="shared" si="5"/>
+        <v>3.9075000000000024</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>B11</f>
+        <f t="shared" si="3"/>
         <v>ctof</v>
       </c>
       <c r="J11" s="5">
-        <f>1000/K11</f>
-        <v>2167.7302996670369</v>
+        <f t="shared" si="4"/>
+        <v>2559.1810620601368</v>
       </c>
       <c r="K11" s="5">
-        <f>D11-D10</f>
-        <v>0.46131199999999994</v>
+        <f t="shared" si="6"/>
+        <v>0.3907500000000006</v>
       </c>
       <c r="L11" s="2">
         <f>H11/$C$23</f>
-        <v>9.553940147043594E-4</v>
+        <v>6.7922383358625011E-4</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -832,43 +835,43 @@
         <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>1.5246</v>
+        <v>27.778099999999998</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="0"/>
-        <v>3.0491999999999999</v>
+        <v>2.7778099999999997</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="1"/>
-        <v>327.95487340941889</v>
+        <v>359.99582404844108</v>
       </c>
       <c r="F12" s="5">
-        <f>D12*$E$5/1000</f>
-        <v>15.246</v>
+        <f t="shared" si="2"/>
+        <v>27.778099999999995</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="2"/>
-        <v>6.3150046598322452E-3</v>
+        <f>C12/C$23</f>
+        <v>4.8285470433121437E-3</v>
       </c>
       <c r="H12" s="1">
-        <f>C12-C11</f>
-        <v>0.31603000000000003</v>
+        <f t="shared" si="5"/>
+        <v>3.7266999999999975</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>B12</f>
+        <f t="shared" si="3"/>
         <v>cnd</v>
       </c>
       <c r="J12" s="5">
-        <f>1000/K12</f>
-        <v>1582.1282789608579</v>
+        <f t="shared" si="4"/>
+        <v>2683.3391472348235</v>
       </c>
       <c r="K12" s="5">
-        <f>D12-D11</f>
-        <v>0.63206000000000007</v>
+        <f t="shared" si="6"/>
+        <v>0.37266999999999939</v>
       </c>
       <c r="L12" s="2">
         <f>H12/$C$23</f>
-        <v>1.3090193641917781E-3</v>
+        <v>6.4779615115185532E-4</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -878,43 +881,43 @@
         <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>17.803799999999999</v>
+        <v>354.774</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="0"/>
-        <v>35.607599999999998</v>
+        <v>35.477400000000003</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="1"/>
-        <v>28.083892202788171</v>
+        <v>28.186958458060623</v>
       </c>
       <c r="F13" s="5">
-        <f>D13*$E$5/1000</f>
-        <v>178.03800000000001</v>
+        <f t="shared" si="2"/>
+        <v>354.77400000000006</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="2"/>
-        <v>7.3744641192917043E-2</v>
+        <f>C13/C$23</f>
+        <v>6.1668830796347572E-2</v>
       </c>
       <c r="H13" s="1">
-        <f>C13-C12</f>
-        <v>16.279199999999999</v>
+        <f t="shared" si="5"/>
+        <v>326.99590000000001</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>B13</f>
+        <f t="shared" si="3"/>
         <v>solenoid</v>
       </c>
       <c r="J13" s="5">
-        <f>1000/K13</f>
-        <v>30.714040001965699</v>
+        <f t="shared" si="4"/>
+        <v>30.58142319215623</v>
       </c>
       <c r="K13" s="5">
-        <f>D13-D12</f>
-        <v>32.558399999999999</v>
+        <f t="shared" si="6"/>
+        <v>32.699590000000001</v>
       </c>
       <c r="L13" s="2">
         <f>H13/$C$23</f>
-        <v>6.74296365330848E-2</v>
+        <v>5.6840283753035431E-2</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -924,43 +927,43 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>29.115100000000002</v>
+        <v>585.20299999999997</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="0"/>
-        <v>58.230200000000004</v>
+        <v>58.520299999999999</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="1"/>
-        <v>17.173219394747054</v>
+        <v>17.088087381643636</v>
       </c>
       <c r="F14" s="5">
-        <f>D14*$E$5/1000</f>
-        <v>291.15100000000001</v>
+        <f t="shared" si="2"/>
+        <v>585.20299999999997</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="2"/>
-        <v>0.12059687273480377</v>
+        <f>C14/C$23</f>
+        <v>0.10172330776357622</v>
       </c>
       <c r="H14" s="1">
-        <f>C14-C13</f>
-        <v>11.311300000000003</v>
+        <f t="shared" si="5"/>
+        <v>230.42899999999997</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>B14</f>
+        <f t="shared" si="3"/>
         <v>mm</v>
       </c>
       <c r="J14" s="5">
-        <f>1000/K14</f>
-        <v>44.203584026592864</v>
+        <f t="shared" si="4"/>
+        <v>43.397315442066763</v>
       </c>
       <c r="K14" s="5">
-        <f>D14-D13</f>
-        <v>22.622600000000006</v>
+        <f t="shared" si="6"/>
+        <v>23.042899999999996</v>
       </c>
       <c r="L14" s="2">
         <f>H14/$C$23</f>
-        <v>4.6852231541886724E-2</v>
+        <v>4.0054476967228636E-2</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -970,319 +973,319 @@
         <v>10</v>
       </c>
       <c r="C15" s="1">
-        <v>42.107199999999999</v>
+        <v>807.851</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="0"/>
-        <v>84.214399999999998</v>
+        <v>80.7851</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="1"/>
-        <v>11.874453775126344</v>
+        <v>12.378520296440804</v>
       </c>
       <c r="F15" s="5">
-        <f>D15*$E$5/1000</f>
-        <v>421.072</v>
+        <f t="shared" si="2"/>
+        <v>807.851</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="2"/>
-        <v>0.17441110075592833</v>
+        <f>C15/C$23</f>
+        <v>0.14042524713665652</v>
       </c>
       <c r="H15" s="1">
-        <f>C15-C14</f>
-        <v>12.992099999999997</v>
+        <f t="shared" si="5"/>
+        <v>222.64800000000002</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>B15</f>
+        <f t="shared" si="3"/>
         <v>htcc</v>
       </c>
       <c r="J15" s="5">
-        <f>1000/K15</f>
-        <v>38.4849254546994</v>
+        <f t="shared" si="4"/>
+        <v>44.913944881606838</v>
       </c>
       <c r="K15" s="5">
-        <f>D15-D14</f>
-        <v>25.984199999999994</v>
+        <f t="shared" si="6"/>
+        <v>22.264800000000001</v>
       </c>
       <c r="L15" s="2">
         <f>H15/$C$23</f>
-        <v>5.3814228021124559E-2</v>
+        <v>3.8701939373080314E-2</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1">
-        <v>60.048200000000001</v>
+        <v>1805.18</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="0"/>
-        <v>120.0964</v>
+        <v>180.518</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="1"/>
-        <v>8.326644262442505</v>
+        <v>5.5396137781273884</v>
       </c>
       <c r="F16" s="5">
-        <f>D16*$E$5/1000</f>
-        <v>600.48199999999997</v>
+        <f t="shared" si="2"/>
+        <v>1805.18</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="2"/>
-        <v>0.24872403437920679</v>
+        <f>C16/C$23</f>
+        <v>0.31378663593428696</v>
       </c>
       <c r="H16" s="1">
-        <f>C16-C15</f>
-        <v>17.941000000000003</v>
+        <f t="shared" si="5"/>
+        <v>997.32900000000006</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>B16</f>
-        <v>dc</v>
+        <f t="shared" si="3"/>
+        <v>torus</v>
       </c>
       <c r="J16" s="5">
-        <f>1000/K16</f>
-        <v>27.869126581572928</v>
+        <f t="shared" si="4"/>
+        <v>10.026781533475914</v>
       </c>
       <c r="K16" s="5">
-        <f>D16-D15</f>
-        <v>35.882000000000005</v>
+        <f t="shared" si="6"/>
+        <v>99.732900000000001</v>
       </c>
       <c r="L16" s="2">
         <f>H16/$C$23</f>
-        <v>7.4312933623278454E-2</v>
+        <v>0.17336138879763041</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>41.963000000000001</v>
+        <v>1995.62</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="0"/>
-        <v>83.926000000000002</v>
+        <v>199.56200000000001</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="1"/>
-        <v>11.915258680265948</v>
+        <v>5.0109740331325607</v>
       </c>
       <c r="F17" s="5">
-        <f>D17*$E$5/1000</f>
-        <v>419.63</v>
+        <f t="shared" si="2"/>
+        <v>1995.6200000000003</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="2"/>
-        <v>0.17381381381381381</v>
+        <f>C17/C$23</f>
+        <v>0.34688999789670927</v>
       </c>
       <c r="H17" s="1">
-        <f>C17-C16</f>
-        <v>-18.0852</v>
+        <f t="shared" si="5"/>
+        <v>190.43999999999983</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>B17</f>
-        <v>torus</v>
+        <f t="shared" si="3"/>
+        <v>rich</v>
       </c>
       <c r="J17" s="5">
-        <f>1000/K17</f>
-        <v>-27.646915710083384</v>
+        <f t="shared" si="4"/>
+        <v>52.509976895610137</v>
       </c>
       <c r="K17" s="5">
-        <f>D17-D16</f>
-        <v>-36.170400000000001</v>
+        <f t="shared" si="6"/>
+        <v>19.044000000000011</v>
       </c>
       <c r="L17" s="2">
         <f>H17/$C$23</f>
-        <v>-7.4910220565392982E-2</v>
+        <v>3.3103361962422334E-2</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1">
-        <v>63.328899999999997</v>
+        <v>2249.58</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="0"/>
-        <v>126.65779999999999</v>
+        <v>224.958</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="1"/>
-        <v>7.8952895123711295</v>
+        <v>4.4452742289671852</v>
       </c>
       <c r="F18" s="5">
-        <f>D18*$E$5/1000</f>
-        <v>633.28899999999999</v>
+        <f t="shared" si="2"/>
+        <v>2249.58</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="2"/>
-        <v>0.26231293362327845</v>
+        <f>C18/C$23</f>
+        <v>0.39103476687369304</v>
       </c>
       <c r="H18" s="1">
         <f>C18-C17</f>
-        <v>21.365899999999996</v>
+        <v>253.96000000000004</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>B18</f>
-        <v>ft</v>
+        <f t="shared" si="3"/>
+        <v>ltcc</v>
       </c>
       <c r="J18" s="5">
-        <f>1000/K18</f>
-        <v>23.401775726742148</v>
+        <f t="shared" si="4"/>
+        <v>39.376279729091216</v>
       </c>
       <c r="K18" s="5">
         <f>D18-D17</f>
-        <v>42.731799999999993</v>
+        <v>25.395999999999987</v>
       </c>
       <c r="L18" s="2">
         <f>H18/$C$23</f>
-        <v>8.8499119809464621E-2</v>
+        <v>4.4144768976983745E-2</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1">
-        <v>58.969000000000001</v>
+        <v>2315.1999999999998</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="0"/>
-        <v>117.938</v>
+        <v>231.52</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="1"/>
-        <v>8.4790313554579519</v>
+        <v>4.3192812715964068</v>
       </c>
       <c r="F19" s="5">
-        <f>D19*$E$5/1000</f>
-        <v>589.69000000000005</v>
+        <f t="shared" si="2"/>
+        <v>2315.1999999999998</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="2"/>
-        <v>0.24425390908149527</v>
+        <f>C19/C$23</f>
+        <v>0.40244120781033527</v>
       </c>
       <c r="H19" s="1">
-        <f>C19-C18</f>
-        <v>-4.3598999999999961</v>
+        <f t="shared" si="5"/>
+        <v>65.619999999999891</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>B19</f>
-        <v>rich</v>
+        <f t="shared" si="3"/>
+        <v>ftof</v>
       </c>
       <c r="J19" s="5">
-        <f>1000/K19</f>
-        <v>-114.68152939287609</v>
+        <f t="shared" si="4"/>
+        <v>152.39256324291347</v>
       </c>
       <c r="K19" s="5">
-        <f>D19-D18</f>
-        <v>-8.7197999999999922</v>
+        <f t="shared" si="6"/>
+        <v>6.5620000000000118</v>
       </c>
       <c r="L19" s="2">
         <f>H19/$C$23</f>
-        <v>-1.8059024541783146E-2</v>
+        <v>1.1406440936642259E-2</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1">
-        <v>61.149000000000001</v>
+        <v>2315.1999999999998</v>
       </c>
       <c r="D20" s="5">
         <f t="shared" si="0"/>
-        <v>122.298</v>
+        <v>231.52</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="1"/>
-        <v>8.1767485976876149</v>
+        <v>4.3192812715964068</v>
       </c>
       <c r="F20" s="5">
-        <f>D20*$E$5/1000</f>
-        <v>611.49</v>
+        <f t="shared" si="2"/>
+        <v>2315.1999999999998</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.25328362845604224</v>
+        <f>C20/C$23</f>
+        <v>0.40244120781033527</v>
       </c>
       <c r="H20" s="1">
-        <f>C20-C19</f>
-        <v>2.1799999999999997</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>B20</f>
-        <v>ltcc</v>
-      </c>
-      <c r="J20" s="5">
-        <f>1000/K20</f>
-        <v>229.35779816513764</v>
+        <f t="shared" si="3"/>
+        <v>ft</v>
+      </c>
+      <c r="J20" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="K20" s="5">
-        <f>D20-D19</f>
-        <v>4.3599999999999994</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="L20" s="2">
         <f>H20/$C$23</f>
-        <v>9.0297193745469597E-3</v>
+        <v>0</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1">
-        <v>63.328899999999997</v>
+        <v>2798.42</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="0"/>
-        <v>126.65779999999999</v>
+        <f>1000*C21/$C$5</f>
+        <v>279.84199999999998</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="1"/>
-        <v>7.8952895123711295</v>
+        <f>$C$5/C21</f>
+        <v>3.573445015401548</v>
       </c>
       <c r="F21" s="5">
         <f>D21*$E$5/1000</f>
-        <v>633.28899999999999</v>
+        <v>2798.42</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="2"/>
-        <v>0.26231293362327845</v>
+        <f>C21/C$23</f>
+        <v>0.48643725153792267</v>
       </c>
       <c r="H21" s="1">
         <f>C21-C20</f>
-        <v>2.1798999999999964</v>
+        <v>483.22000000000025</v>
       </c>
       <c r="I21" s="1" t="str">
         <f>B21</f>
-        <v>ftof</v>
+        <v>dc</v>
       </c>
       <c r="J21" s="5">
         <f>1000/K21</f>
-        <v>229.36831964769064</v>
+        <v>20.694507677662358</v>
       </c>
       <c r="K21" s="5">
         <f>D21-D20</f>
-        <v>4.3597999999999928</v>
+        <v>48.321999999999974</v>
       </c>
       <c r="L21" s="2">
         <f>H21/$C$23</f>
-        <v>9.0293051672361863E-3</v>
+        <v>8.3996043727587386E-2</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1292,43 +1295,43 @@
         <v>17</v>
       </c>
       <c r="C22" s="1">
-        <v>158.65100000000001</v>
+        <v>4188.1499999999996</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="0"/>
-        <v>317.30200000000002</v>
+        <v>418.81499999999994</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="1"/>
-        <v>3.1515716888012051</v>
+        <v>2.387689075128637</v>
       </c>
       <c r="F22" s="5">
-        <f>D22*$E$5/1000</f>
-        <v>1586.51</v>
+        <f t="shared" si="2"/>
+        <v>4188.1499999999996</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="2"/>
-        <v>0.65714404059231646</v>
+        <f>C22/C$23</f>
+        <v>0.72800800988720438</v>
       </c>
       <c r="H22" s="1">
         <f>C22-C21</f>
-        <v>95.322100000000006</v>
+        <v>1389.7299999999996</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>B22</f>
+        <f t="shared" si="3"/>
         <v>pcal</v>
       </c>
       <c r="J22" s="5">
-        <f>1000/K22</f>
-        <v>5.2453733184644484</v>
+        <f t="shared" si="4"/>
+        <v>7.1956423190116086</v>
       </c>
       <c r="K22" s="5">
         <f>D22-D21</f>
-        <v>190.64420000000001</v>
+        <v>138.97299999999996</v>
       </c>
       <c r="L22" s="2">
         <f>H22/$C$23</f>
-        <v>0.394831106969038</v>
+        <v>0.24157075834928174</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1338,43 +1341,43 @@
         <v>18</v>
       </c>
       <c r="C23" s="1">
-        <v>241.42500000000001</v>
+        <v>5752.89</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="0"/>
-        <v>482.85</v>
+        <v>575.28899999999999</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="1"/>
-        <v>2.0710365537951745</v>
+        <v>1.7382567718138187</v>
       </c>
       <c r="F23" s="5">
-        <f>D23*$E$5/1000</f>
-        <v>2414.25</v>
+        <f t="shared" si="2"/>
+        <v>5752.89</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="2"/>
+        <f>C23/C$23</f>
         <v>1</v>
       </c>
       <c r="H23" s="1">
-        <f>C23-C22</f>
-        <v>82.774000000000001</v>
+        <f t="shared" si="5"/>
+        <v>1564.7400000000007</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>B23</f>
+        <f t="shared" si="3"/>
         <v>ecAll</v>
       </c>
       <c r="J23" s="5">
-        <f>1000/K23</f>
-        <v>6.0405441322154303</v>
+        <f t="shared" si="4"/>
+        <v>6.3908380945077115</v>
       </c>
       <c r="K23" s="5">
-        <f>D23-D22</f>
-        <v>165.548</v>
+        <f t="shared" si="6"/>
+        <v>156.47400000000005</v>
       </c>
       <c r="L23" s="2">
         <f>H23/$C$23</f>
-        <v>0.34285595940768354</v>
+        <v>0.27199199011279557</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>

</xml_diff>

<commit_message>
corrected ftof and ltcc numbers
</commit_message>
<xml_diff>
--- a/benchmarks/template.xlsx
+++ b/benchmarks/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/projects/gemc/clas12Tags/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7DC960-D85F-4245-B0E4-63A45C84DF13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F189F6D-8A11-2840-A10E-CAFE36F50376}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10040" yWindow="2780" windowWidth="44280" windowHeight="31240" xr2:uid="{28AA30A8-E2EF-AD44-AC50-0F7BDEF7D56D}"/>
+    <workbookView xWindow="17200" yWindow="1820" windowWidth="41420" windowHeight="27060" xr2:uid="{28AA30A8-E2EF-AD44-AC50-0F7BDEF7D56D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
   <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,21 +605,21 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="1">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="F5" s="7">
         <f>SUM(F9:F23)</f>
-        <v>25251.930499999999</v>
+        <v>11835.666289999999</v>
       </c>
       <c r="G5" s="7">
         <f>F5/3600</f>
-        <v>7.0144251388888881</v>
+        <v>3.2876850805555553</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -697,27 +697,27 @@
         <v>19</v>
       </c>
       <c r="C9" s="1">
-        <v>11.889099999999999</v>
+        <v>6.0090899999999996</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" ref="D9:D23" si="0">1000*C9/$C$5</f>
-        <v>1.1889099999999999</v>
+        <v>1.2018179999999998</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" ref="E9:E23" si="1">$C$5/C9</f>
-        <v>841.10655979005992</v>
+        <v>832.07274312749519</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" ref="F9:F23" si="2">D9*$E$5/1000</f>
-        <v>11.889099999999999</v>
+        <v>6.0090899999999996</v>
       </c>
       <c r="G9" s="2">
         <f>C9/C$23</f>
-        <v>2.0666308585771671E-3</v>
+        <v>2.0436857212820371E-3</v>
       </c>
       <c r="H9" s="1">
         <f>C9</f>
-        <v>11.889099999999999</v>
+        <v>6.0090899999999996</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" ref="I9:I23" si="3">B9</f>
@@ -725,15 +725,15 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" ref="J9:J23" si="4">1000/K9</f>
-        <v>841.10655979005992</v>
+        <v>832.0727431274953</v>
       </c>
       <c r="K9" s="5">
         <f>D9</f>
-        <v>1.1889099999999999</v>
+        <v>1.2018179999999998</v>
       </c>
       <c r="L9" s="2">
         <f>H9/$C$23</f>
-        <v>2.0666308585771671E-3</v>
+        <v>2.0436857212820371E-3</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -743,27 +743,27 @@
         <v>5</v>
       </c>
       <c r="C10" s="1">
-        <v>20.143899999999999</v>
+        <v>10.638</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="0"/>
-        <v>2.0143899999999997</v>
+        <v>2.1276000000000002</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="1"/>
-        <v>496.42819910742213</v>
+        <v>470.01316036849033</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>20.143899999999999</v>
+        <v>10.638</v>
       </c>
       <c r="G10" s="2">
         <f>C10/C$23</f>
-        <v>3.5015270585740379E-3</v>
+        <v>3.6179735538988951E-3</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10:H23" si="5">C10-C9</f>
-        <v>8.2547999999999995</v>
+        <v>4.6289100000000003</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="3"/>
@@ -771,15 +771,15 @@
       </c>
       <c r="J10" s="5">
         <f t="shared" si="4"/>
-        <v>1211.4163880408978</v>
+        <v>1080.1679012985774</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" ref="K10:K23" si="6">D10-D9</f>
-        <v>0.82547999999999977</v>
+        <v>0.92578200000000033</v>
       </c>
       <c r="L10" s="2">
         <f>H10/$C$23</f>
-        <v>1.434896199996871E-3</v>
+        <v>1.574287832616858E-3</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -789,27 +789,27 @@
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>24.051400000000001</v>
+        <v>12.486000000000001</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="0"/>
-        <v>2.4051400000000003</v>
+        <v>2.4971999999999999</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="1"/>
-        <v>415.77621261132407</v>
+        <v>400.44850232260131</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>24.051400000000001</v>
+        <v>12.486000000000001</v>
       </c>
       <c r="G11" s="2">
         <f>C11/C$23</f>
-        <v>4.1807508921602879E-3</v>
+        <v>4.2464765739783422E-3</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="5"/>
-        <v>3.9075000000000024</v>
+        <v>1.8480000000000008</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="3"/>
@@ -817,15 +817,15 @@
       </c>
       <c r="J11" s="5">
         <f t="shared" si="4"/>
-        <v>2559.1810620601368</v>
+        <v>2705.6277056277077</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="6"/>
-        <v>0.3907500000000006</v>
+        <v>0.36959999999999971</v>
       </c>
       <c r="L11" s="2">
         <f>H11/$C$23</f>
-        <v>6.7922383358625011E-4</v>
+        <v>6.2850302007944731E-4</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -835,27 +835,27 @@
         <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>27.778099999999998</v>
+        <v>13.5182</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="0"/>
-        <v>2.7778099999999997</v>
+        <v>2.70364</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="1"/>
-        <v>359.99582404844108</v>
+        <v>369.87172848456157</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>27.778099999999995</v>
+        <v>13.5182</v>
       </c>
       <c r="G12" s="2">
         <f>C12/C$23</f>
-        <v>4.8285470433121437E-3</v>
+        <v>4.5975267998041025E-3</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="5"/>
-        <v>3.7266999999999975</v>
+        <v>1.0321999999999996</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="3"/>
@@ -863,15 +863,15 @@
       </c>
       <c r="J12" s="5">
         <f t="shared" si="4"/>
-        <v>2683.3391472348235</v>
+        <v>4844.0224762642856</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="6"/>
-        <v>0.37266999999999939</v>
+        <v>0.20644000000000018</v>
       </c>
       <c r="L12" s="2">
         <f>H12/$C$23</f>
-        <v>6.4779615115185532E-4</v>
+        <v>3.5105022582576027E-4</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -881,27 +881,27 @@
         <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>354.774</v>
+        <v>183.06899999999999</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="0"/>
-        <v>35.477400000000003</v>
+        <v>36.613799999999998</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="1"/>
-        <v>28.186958458060623</v>
+        <v>27.312106364267027</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>354.77400000000006</v>
+        <v>183.06899999999999</v>
       </c>
       <c r="G13" s="2">
         <f>C13/C$23</f>
-        <v>6.1668830796347572E-2</v>
+        <v>6.2261590575175482E-2</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="5"/>
-        <v>326.99590000000001</v>
+        <v>169.55079999999998</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="3"/>
@@ -909,15 +909,15 @@
       </c>
       <c r="J13" s="5">
         <f t="shared" si="4"/>
-        <v>30.58142319215623</v>
+        <v>29.489686866708976</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="6"/>
-        <v>32.699590000000001</v>
+        <v>33.910159999999998</v>
       </c>
       <c r="L13" s="2">
         <f>H13/$C$23</f>
-        <v>5.6840283753035431E-2</v>
+        <v>5.766406377537138E-2</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -927,27 +927,27 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>585.20299999999997</v>
+        <v>313.517</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="0"/>
-        <v>58.520299999999999</v>
+        <v>62.703400000000002</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="1"/>
-        <v>17.088087381643636</v>
+        <v>15.948098508214866</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>585.20299999999997</v>
+        <v>313.517</v>
       </c>
       <c r="G14" s="2">
         <f>C14/C$23</f>
-        <v>0.10172330776357622</v>
+        <v>0.10662682973281819</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="5"/>
-        <v>230.42899999999997</v>
+        <v>130.44800000000001</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="3"/>
@@ -955,15 +955,15 @@
       </c>
       <c r="J14" s="5">
         <f t="shared" si="4"/>
-        <v>43.397315442066763</v>
+        <v>38.329449282472702</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="6"/>
-        <v>23.042899999999996</v>
+        <v>26.089600000000004</v>
       </c>
       <c r="L14" s="2">
         <f>H14/$C$23</f>
-        <v>4.0054476967228636E-2</v>
+        <v>4.4365239157642705E-2</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -973,27 +973,27 @@
         <v>10</v>
       </c>
       <c r="C15" s="1">
-        <v>807.851</v>
+        <v>415.98899999999998</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="0"/>
-        <v>80.7851</v>
+        <v>83.197800000000001</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="1"/>
-        <v>12.378520296440804</v>
+        <v>12.019548593833012</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>807.851</v>
+        <v>415.98899999999998</v>
       </c>
       <c r="G15" s="2">
         <f>C15/C$23</f>
-        <v>0.14042524713665652</v>
+        <v>0.14147745823583827</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="5"/>
-        <v>222.64800000000002</v>
+        <v>102.47199999999998</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1001,15 +1001,15 @@
       </c>
       <c r="J15" s="5">
         <f t="shared" si="4"/>
-        <v>44.913944881606838</v>
+        <v>48.793816847529087</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="6"/>
-        <v>22.264800000000001</v>
+        <v>20.494399999999999</v>
       </c>
       <c r="L15" s="2">
         <f>H15/$C$23</f>
-        <v>3.8701939373080314E-2</v>
+        <v>3.4850628503020072E-2</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1019,27 +1019,27 @@
         <v>12</v>
       </c>
       <c r="C16" s="1">
-        <v>1805.18</v>
+        <v>641.35199999999998</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="0"/>
-        <v>180.518</v>
+        <v>128.2704</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="1"/>
-        <v>5.5396137781273884</v>
+        <v>7.796030884755953</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>1805.18</v>
+        <v>641.35199999999998</v>
       </c>
       <c r="G16" s="2">
         <f>C16/C$23</f>
-        <v>0.31378663593428696</v>
+        <v>0.21812319747510472</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="5"/>
-        <v>997.32900000000006</v>
+        <v>225.363</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1047,245 +1047,245 @@
       </c>
       <c r="J16" s="5">
         <f t="shared" si="4"/>
-        <v>10.026781533475914</v>
+        <v>22.186428118191543</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="6"/>
-        <v>99.732900000000001</v>
+        <v>45.072599999999994</v>
       </c>
       <c r="L16" s="2">
         <f>H16/$C$23</f>
-        <v>0.17336138879763041</v>
+        <v>7.6645739239266472E-2</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
-        <v>1995.62</v>
+        <v>693.80200000000002</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="0"/>
-        <v>199.56200000000001</v>
+        <v>138.7604</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="1"/>
-        <v>5.0109740331325607</v>
+        <v>7.2066670318044626</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>1995.6200000000003</v>
+        <v>693.80200000000002</v>
       </c>
       <c r="G17" s="2">
         <f>C17/C$23</f>
-        <v>0.34688999789670927</v>
+        <v>0.23596139195733798</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="5"/>
-        <v>190.43999999999983</v>
+        <v>52.450000000000045</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>rich</v>
+        <v>ft</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="4"/>
-        <v>52.509976895610137</v>
+        <v>95.328884652049481</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="6"/>
-        <v>19.044000000000011</v>
+        <v>10.490000000000009</v>
       </c>
       <c r="L17" s="2">
         <f>H17/$C$23</f>
-        <v>3.3103361962422334E-2</v>
+        <v>1.7838194482233241E-2</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1">
-        <v>2249.58</v>
+        <v>935.13599999999997</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="0"/>
-        <v>224.958</v>
+        <v>187.02719999999999</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="1"/>
-        <v>4.4452742289671852</v>
+        <v>5.3468158642165422</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="2"/>
-        <v>2249.58</v>
+        <v>935.13599999999997</v>
       </c>
       <c r="G18" s="2">
         <f>C18/C$23</f>
-        <v>0.39103476687369304</v>
+        <v>0.31803885291396849</v>
       </c>
       <c r="H18" s="1">
         <f>C18-C17</f>
-        <v>253.96000000000004</v>
+        <v>241.33399999999995</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ltcc</v>
+        <v>dc</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="4"/>
-        <v>39.376279729091216</v>
+        <v>20.718174811671794</v>
       </c>
       <c r="K18" s="5">
         <f>D18-D17</f>
-        <v>25.395999999999987</v>
+        <v>48.266799999999989</v>
       </c>
       <c r="L18" s="2">
         <f>H18/$C$23</f>
-        <v>4.4144768976983745E-2</v>
+        <v>8.2077460956630544E-2</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1">
-        <v>2315.1999999999998</v>
+        <v>1053.01</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="0"/>
-        <v>231.52</v>
+        <v>210.602</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="1"/>
-        <v>4.3192812715964068</v>
+        <v>4.7482929886705731</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="2"/>
-        <v>2315.1999999999998</v>
+        <v>1053.01</v>
       </c>
       <c r="G19" s="2">
         <f>C19/C$23</f>
-        <v>0.40244120781033527</v>
+        <v>0.35812768678239099</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="5"/>
-        <v>65.619999999999891</v>
+        <v>117.87400000000002</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ftof</v>
+        <v>rich</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="4"/>
-        <v>152.39256324291347</v>
+        <v>42.418175339769569</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="6"/>
-        <v>6.5620000000000118</v>
+        <v>23.57480000000001</v>
       </c>
       <c r="L19" s="2">
         <f>H19/$C$23</f>
-        <v>1.1406440936642259E-2</v>
+        <v>4.0088833868422491E-2</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1">
-        <v>2315.1999999999998</v>
+        <v>1190.92</v>
       </c>
       <c r="D20" s="5">
         <f t="shared" si="0"/>
-        <v>231.52</v>
+        <v>238.184</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="1"/>
-        <v>4.3192812715964068</v>
+        <v>4.1984348234977995</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="2"/>
-        <v>2315.1999999999998</v>
+        <v>1190.92</v>
       </c>
       <c r="G20" s="2">
         <f>C20/C$23</f>
-        <v>0.40244120781033527</v>
+        <v>0.40503074495293029</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>137.91000000000008</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>ft</v>
-      </c>
-      <c r="J20" s="5" t="e">
+        <v>ltcc</v>
+      </c>
+      <c r="J20" s="5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>36.255528968167653</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>27.581999999999994</v>
       </c>
       <c r="L20" s="2">
         <f>H20/$C$23</f>
-        <v>0</v>
+        <v>4.6903058170539288E-2</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1">
-        <v>2798.42</v>
+        <v>1247.4000000000001</v>
       </c>
       <c r="D21" s="5">
         <f>1000*C21/$C$5</f>
-        <v>279.84199999999998</v>
+        <v>249.48</v>
       </c>
       <c r="E21" s="5">
         <f>$C$5/C21</f>
-        <v>3.573445015401548</v>
+        <v>4.0083373416706749</v>
       </c>
       <c r="F21" s="5">
         <f>D21*$E$5/1000</f>
-        <v>2798.42</v>
+        <v>1247.4000000000001</v>
       </c>
       <c r="G21" s="2">
         <f>C21/C$23</f>
-        <v>0.48643725153792267</v>
+        <v>0.42423953855362684</v>
       </c>
       <c r="H21" s="1">
         <f>C21-C20</f>
-        <v>483.22000000000025</v>
+        <v>56.480000000000018</v>
       </c>
       <c r="I21" s="1" t="str">
         <f>B21</f>
-        <v>dc</v>
+        <v>ftof</v>
       </c>
       <c r="J21" s="5">
         <f>1000/K21</f>
-        <v>20.694507677662358</v>
+        <v>88.526912181303175</v>
       </c>
       <c r="K21" s="5">
         <f>D21-D20</f>
-        <v>48.321999999999974</v>
+        <v>11.295999999999992</v>
       </c>
       <c r="L21" s="2">
         <f>H21/$C$23</f>
-        <v>8.3996043727587386E-2</v>
+        <v>1.9208793600696529E-2</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1295,27 +1295,27 @@
         <v>17</v>
       </c>
       <c r="C22" s="1">
-        <v>4188.1499999999996</v>
+        <v>2178.5</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="0"/>
-        <v>418.81499999999994</v>
+        <v>435.7</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="1"/>
-        <v>2.387689075128637</v>
+        <v>2.2951572182694515</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="2"/>
-        <v>4188.1499999999996</v>
+        <v>2178.5</v>
       </c>
       <c r="G22" s="2">
         <f>C22/C$23</f>
-        <v>0.72800800988720438</v>
+        <v>0.74090575175491102</v>
       </c>
       <c r="H22" s="1">
         <f>C22-C21</f>
-        <v>1389.7299999999996</v>
+        <v>931.09999999999991</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1323,15 +1323,15 @@
       </c>
       <c r="J22" s="5">
         <f t="shared" si="4"/>
-        <v>7.1956423190116086</v>
+        <v>5.3699924820105256</v>
       </c>
       <c r="K22" s="5">
         <f>D22-D21</f>
-        <v>138.97299999999996</v>
+        <v>186.22</v>
       </c>
       <c r="L22" s="2">
         <f>H22/$C$23</f>
-        <v>0.24157075834928174</v>
+        <v>0.31666621320128419</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1341,19 +1341,19 @@
         <v>18</v>
       </c>
       <c r="C23" s="1">
-        <v>5752.89</v>
+        <v>2940.32</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="0"/>
-        <v>575.28899999999999</v>
+        <v>588.06399999999996</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="1"/>
-        <v>1.7382567718138187</v>
+        <v>1.7004951841976383</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="2"/>
-        <v>5752.89</v>
+        <v>2940.32</v>
       </c>
       <c r="G23" s="2">
         <f>C23/C$23</f>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" si="5"/>
-        <v>1564.7400000000007</v>
+        <v>761.82000000000016</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1369,15 +1369,15 @@
       </c>
       <c r="J23" s="5">
         <f t="shared" si="4"/>
-        <v>6.3908380945077115</v>
+        <v>6.5632301593552294</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="6"/>
-        <v>156.47400000000005</v>
+        <v>152.36399999999998</v>
       </c>
       <c r="L23" s="2">
         <f>H23/$C$23</f>
-        <v>0.27199199011279557</v>
+        <v>0.25909424824508903</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>

</xml_diff>

<commit_message>
added total column for rates
</commit_message>
<xml_diff>
--- a/benchmarks/template.xlsx
+++ b/benchmarks/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/projects/gemc/clas12Tags/benchmarks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7662385C-8F50-DD4A-B61C-B7F83EA153DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4418AA9-E265-1641-8A9C-0B2A1FD65C15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20180" yWindow="1460" windowWidth="41420" windowHeight="27060" xr2:uid="{28AA30A8-E2EF-AD44-AC50-0F7BDEF7D56D}"/>
   </bookViews>
@@ -225,13 +225,13 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -552,7 +552,7 @@
   <dimension ref="B2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,19 +568,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="2:14" ht="26" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -647,19 +647,19 @@
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
@@ -715,7 +715,7 @@
         <v>6.0090899999999996</v>
       </c>
       <c r="G9" s="2">
-        <f>C9/C$23</f>
+        <f t="shared" ref="G9:G23" si="3">C9/C$23</f>
         <v>2.0436857212820371E-3</v>
       </c>
       <c r="H9" s="1">
@@ -723,19 +723,19 @@
         <v>6.0090899999999996</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f t="shared" ref="I9:I23" si="3">B9</f>
+        <f t="shared" ref="I9:I23" si="4">B9</f>
         <v>target</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" ref="J9:J23" si="4">1000/K9</f>
+        <f t="shared" ref="J9:J24" si="5">1000/K9</f>
         <v>832.0727431274953</v>
       </c>
       <c r="K9" s="5">
         <f>D9</f>
         <v>1.2018179999999998</v>
       </c>
-      <c r="L9" s="10">
-        <f>H9/$C$23</f>
+      <c r="L9" s="8">
+        <f t="shared" ref="L9:L23" si="6">H9/$C$23</f>
         <v>2.0436857212820371E-3</v>
       </c>
       <c r="M9" s="1"/>
@@ -761,27 +761,27 @@
         <v>10.638</v>
       </c>
       <c r="G10" s="2">
-        <f>C10/C$23</f>
+        <f t="shared" si="3"/>
         <v>3.6179735538988951E-3</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10:H23" si="5">C10-C9</f>
+        <f t="shared" ref="H10:H23" si="7">C10-C9</f>
         <v>4.6289100000000003</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>svt</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1080.1679012985774</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" ref="K10:K23" si="6">D10-D9</f>
+        <f t="shared" ref="K10:K23" si="8">D10-D9</f>
         <v>0.92578200000000033</v>
       </c>
-      <c r="L10" s="10">
-        <f>H10/$C$23</f>
+      <c r="L10" s="8">
+        <f t="shared" si="6"/>
         <v>1.574287832616858E-3</v>
       </c>
       <c r="M10" s="1"/>
@@ -807,27 +807,27 @@
         <v>12.486000000000001</v>
       </c>
       <c r="G11" s="2">
-        <f>C11/C$23</f>
+        <f t="shared" si="3"/>
         <v>4.2464765739783422E-3</v>
       </c>
       <c r="H11" s="1">
+        <f t="shared" si="7"/>
+        <v>1.8480000000000008</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ctof</v>
+      </c>
+      <c r="J11" s="5">
         <f t="shared" si="5"/>
-        <v>1.8480000000000008</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ctof</v>
-      </c>
-      <c r="J11" s="5">
-        <f t="shared" si="4"/>
         <v>2705.6277056277077</v>
       </c>
       <c r="K11" s="5">
+        <f t="shared" si="8"/>
+        <v>0.36959999999999971</v>
+      </c>
+      <c r="L11" s="8">
         <f t="shared" si="6"/>
-        <v>0.36959999999999971</v>
-      </c>
-      <c r="L11" s="10">
-        <f>H11/$C$23</f>
         <v>6.2850302007944731E-4</v>
       </c>
       <c r="M11" s="1"/>
@@ -853,27 +853,27 @@
         <v>13.5182</v>
       </c>
       <c r="G12" s="2">
-        <f>C12/C$23</f>
+        <f t="shared" si="3"/>
         <v>4.5975267998041025E-3</v>
       </c>
       <c r="H12" s="1">
+        <f t="shared" si="7"/>
+        <v>1.0321999999999996</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>cnd</v>
+      </c>
+      <c r="J12" s="5">
         <f t="shared" si="5"/>
-        <v>1.0321999999999996</v>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>cnd</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" si="4"/>
         <v>4844.0224762642856</v>
       </c>
       <c r="K12" s="5">
+        <f t="shared" si="8"/>
+        <v>0.20644000000000018</v>
+      </c>
+      <c r="L12" s="8">
         <f t="shared" si="6"/>
-        <v>0.20644000000000018</v>
-      </c>
-      <c r="L12" s="10">
-        <f>H12/$C$23</f>
         <v>3.5105022582576027E-4</v>
       </c>
       <c r="M12" s="1"/>
@@ -899,27 +899,27 @@
         <v>183.06899999999999</v>
       </c>
       <c r="G13" s="2">
-        <f>C13/C$23</f>
+        <f t="shared" si="3"/>
         <v>6.2261590575175482E-2</v>
       </c>
       <c r="H13" s="1">
+        <f t="shared" si="7"/>
+        <v>169.55079999999998</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>solenoid</v>
+      </c>
+      <c r="J13" s="5">
         <f t="shared" si="5"/>
-        <v>169.55079999999998</v>
-      </c>
-      <c r="I13" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>solenoid</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="4"/>
         <v>29.489686866708976</v>
       </c>
       <c r="K13" s="5">
+        <f t="shared" si="8"/>
+        <v>33.910159999999998</v>
+      </c>
+      <c r="L13" s="8">
         <f t="shared" si="6"/>
-        <v>33.910159999999998</v>
-      </c>
-      <c r="L13" s="10">
-        <f>H13/$C$23</f>
         <v>5.766406377537138E-2</v>
       </c>
       <c r="M13" s="1"/>
@@ -945,27 +945,27 @@
         <v>313.517</v>
       </c>
       <c r="G14" s="2">
-        <f>C14/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.10662682973281819</v>
       </c>
       <c r="H14" s="1">
+        <f t="shared" si="7"/>
+        <v>130.44800000000001</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>mm</v>
+      </c>
+      <c r="J14" s="5">
         <f t="shared" si="5"/>
-        <v>130.44800000000001</v>
-      </c>
-      <c r="I14" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>mm</v>
-      </c>
-      <c r="J14" s="5">
-        <f t="shared" si="4"/>
         <v>38.329449282472702</v>
       </c>
       <c r="K14" s="5">
+        <f t="shared" si="8"/>
+        <v>26.089600000000004</v>
+      </c>
+      <c r="L14" s="8">
         <f t="shared" si="6"/>
-        <v>26.089600000000004</v>
-      </c>
-      <c r="L14" s="10">
-        <f>H14/$C$23</f>
         <v>4.4365239157642705E-2</v>
       </c>
       <c r="M14" s="1"/>
@@ -991,27 +991,27 @@
         <v>415.98899999999998</v>
       </c>
       <c r="G15" s="2">
-        <f>C15/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.14147745823583827</v>
       </c>
       <c r="H15" s="1">
+        <f t="shared" si="7"/>
+        <v>102.47199999999998</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>htcc</v>
+      </c>
+      <c r="J15" s="5">
         <f t="shared" si="5"/>
-        <v>102.47199999999998</v>
-      </c>
-      <c r="I15" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>htcc</v>
-      </c>
-      <c r="J15" s="5">
-        <f t="shared" si="4"/>
         <v>48.793816847529087</v>
       </c>
       <c r="K15" s="5">
+        <f t="shared" si="8"/>
+        <v>20.494399999999999</v>
+      </c>
+      <c r="L15" s="8">
         <f t="shared" si="6"/>
-        <v>20.494399999999999</v>
-      </c>
-      <c r="L15" s="10">
-        <f>H15/$C$23</f>
         <v>3.4850628503020072E-2</v>
       </c>
       <c r="M15" s="1"/>
@@ -1037,27 +1037,27 @@
         <v>641.35199999999998</v>
       </c>
       <c r="G16" s="2">
-        <f>C16/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.21812319747510472</v>
       </c>
       <c r="H16" s="1">
+        <f t="shared" si="7"/>
+        <v>225.363</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>torus</v>
+      </c>
+      <c r="J16" s="5">
         <f t="shared" si="5"/>
-        <v>225.363</v>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>torus</v>
-      </c>
-      <c r="J16" s="5">
-        <f t="shared" si="4"/>
         <v>22.186428118191543</v>
       </c>
       <c r="K16" s="5">
+        <f t="shared" si="8"/>
+        <v>45.072599999999994</v>
+      </c>
+      <c r="L16" s="8">
         <f t="shared" si="6"/>
-        <v>45.072599999999994</v>
-      </c>
-      <c r="L16" s="10">
-        <f>H16/$C$23</f>
         <v>7.6645739239266472E-2</v>
       </c>
       <c r="M16" s="1"/>
@@ -1083,27 +1083,27 @@
         <v>693.80200000000002</v>
       </c>
       <c r="G17" s="2">
-        <f>C17/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.23596139195733798</v>
       </c>
       <c r="H17" s="1">
+        <f t="shared" si="7"/>
+        <v>52.450000000000045</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ft</v>
+      </c>
+      <c r="J17" s="5">
         <f t="shared" si="5"/>
-        <v>52.450000000000045</v>
-      </c>
-      <c r="I17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ft</v>
-      </c>
-      <c r="J17" s="5">
-        <f t="shared" si="4"/>
         <v>95.328884652049481</v>
       </c>
       <c r="K17" s="5">
+        <f t="shared" si="8"/>
+        <v>10.490000000000009</v>
+      </c>
+      <c r="L17" s="8">
         <f t="shared" si="6"/>
-        <v>10.490000000000009</v>
-      </c>
-      <c r="L17" s="10">
-        <f>H17/$C$23</f>
         <v>1.7838194482233241E-2</v>
       </c>
       <c r="M17" s="1"/>
@@ -1129,7 +1129,7 @@
         <v>935.13599999999997</v>
       </c>
       <c r="G18" s="2">
-        <f>C18/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.31803885291396849</v>
       </c>
       <c r="H18" s="1">
@@ -1137,19 +1137,19 @@
         <v>241.33399999999995</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>dc</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.718174811671794</v>
       </c>
       <c r="K18" s="5">
         <f>D18-D17</f>
         <v>48.266799999999989</v>
       </c>
-      <c r="L18" s="10">
-        <f>H18/$C$23</f>
+      <c r="L18" s="8">
+        <f t="shared" si="6"/>
         <v>8.2077460956630544E-2</v>
       </c>
       <c r="M18" s="1"/>
@@ -1175,27 +1175,27 @@
         <v>1053.01</v>
       </c>
       <c r="G19" s="2">
-        <f>C19/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.35812768678239099</v>
       </c>
       <c r="H19" s="1">
+        <f t="shared" si="7"/>
+        <v>117.87400000000002</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>rich</v>
+      </c>
+      <c r="J19" s="5">
         <f t="shared" si="5"/>
-        <v>117.87400000000002</v>
-      </c>
-      <c r="I19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>rich</v>
-      </c>
-      <c r="J19" s="5">
-        <f t="shared" si="4"/>
         <v>42.418175339769569</v>
       </c>
       <c r="K19" s="5">
+        <f t="shared" si="8"/>
+        <v>23.57480000000001</v>
+      </c>
+      <c r="L19" s="8">
         <f t="shared" si="6"/>
-        <v>23.57480000000001</v>
-      </c>
-      <c r="L19" s="10">
-        <f>H19/$C$23</f>
         <v>4.0088833868422491E-2</v>
       </c>
       <c r="M19" s="1"/>
@@ -1221,27 +1221,27 @@
         <v>1190.92</v>
       </c>
       <c r="G20" s="2">
-        <f>C20/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.40503074495293029</v>
       </c>
       <c r="H20" s="1">
+        <f t="shared" si="7"/>
+        <v>137.91000000000008</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ltcc</v>
+      </c>
+      <c r="J20" s="5">
         <f t="shared" si="5"/>
-        <v>137.91000000000008</v>
-      </c>
-      <c r="I20" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ltcc</v>
-      </c>
-      <c r="J20" s="5">
-        <f t="shared" si="4"/>
         <v>36.255528968167653</v>
       </c>
       <c r="K20" s="5">
+        <f t="shared" si="8"/>
+        <v>27.581999999999994</v>
+      </c>
+      <c r="L20" s="8">
         <f t="shared" si="6"/>
-        <v>27.581999999999994</v>
-      </c>
-      <c r="L20" s="10">
-        <f>H20/$C$23</f>
         <v>4.6903058170539288E-2</v>
       </c>
       <c r="M20" s="1"/>
@@ -1267,7 +1267,7 @@
         <v>1247.4000000000001</v>
       </c>
       <c r="G21" s="2">
-        <f>C21/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.42423953855362684</v>
       </c>
       <c r="H21" s="1">
@@ -1286,8 +1286,8 @@
         <f>D21-D20</f>
         <v>11.295999999999992</v>
       </c>
-      <c r="L21" s="10">
-        <f>H21/$C$23</f>
+      <c r="L21" s="8">
+        <f t="shared" si="6"/>
         <v>1.9208793600696529E-2</v>
       </c>
       <c r="M21" s="1"/>
@@ -1313,7 +1313,7 @@
         <v>2178.5</v>
       </c>
       <c r="G22" s="2">
-        <f>C22/C$23</f>
+        <f t="shared" si="3"/>
         <v>0.74090575175491102</v>
       </c>
       <c r="H22" s="1">
@@ -1321,19 +1321,19 @@
         <v>931.09999999999991</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>pcal</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.3699924820105256</v>
       </c>
       <c r="K22" s="5">
         <f>D22-D21</f>
         <v>186.22</v>
       </c>
-      <c r="L22" s="10">
-        <f>H22/$C$23</f>
+      <c r="L22" s="8">
+        <f t="shared" si="6"/>
         <v>0.31666621320128419</v>
       </c>
       <c r="M22" s="1"/>
@@ -1359,27 +1359,27 @@
         <v>2940.32</v>
       </c>
       <c r="G23" s="2">
-        <f>C23/C$23</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H23" s="1">
+        <f t="shared" si="7"/>
+        <v>761.82000000000016</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>ecAll</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="5"/>
-        <v>761.82000000000016</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>ecAll</v>
-      </c>
-      <c r="J23" s="5">
-        <f t="shared" si="4"/>
         <v>6.5632301593552294</v>
       </c>
       <c r="K23" s="5">
+        <f t="shared" si="8"/>
+        <v>152.36399999999998</v>
+      </c>
+      <c r="L23" s="8">
         <f t="shared" si="6"/>
-        <v>152.36399999999998</v>
-      </c>
-      <c r="L23" s="10">
-        <f>H23/$C$23</f>
         <v>0.25909424824508903</v>
       </c>
       <c r="M23" s="1"/>
@@ -1392,9 +1392,18 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="J24" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7004951841976386</v>
+      </c>
+      <c r="K24" s="5">
+        <f>SUM(K9:K23)</f>
+        <v>588.06399999999996</v>
+      </c>
+      <c r="L24" s="8">
+        <f>SUM(L9:L23)</f>
+        <v>1</v>
+      </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>

</xml_diff>